<commit_message>
added cable holder & updated parameters
</commit_message>
<xml_diff>
--- a/Drawings/CNC_BOM.xlsx
+++ b/Drawings/CNC_BOM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\development\GitHub\SpindleCarriageForCNC\Drawings\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\development\GitHub\LaserCNCMachine\Drawings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B4CA76-AFF0-411F-8CC7-A3713D01EAE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A131EA4-007E-423B-8E72-9930EC6DBC9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="154">
   <si>
     <t>File</t>
   </si>
@@ -579,6 +579,9 @@
   <si>
     <t>Spacer</t>
   </si>
+  <si>
+    <t>91166A240</t>
+  </si>
 </sst>
 </file>
 
@@ -587,7 +590,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-809]dd\ mmmm\ yyyy;@"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -659,8 +662,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -685,6 +695,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="42">
     <border>
@@ -1212,15 +1227,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="218">
+  <cellXfs count="217">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1716,126 +1732,18 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="19" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="36" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="40" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1843,9 +1751,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="36" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="41" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1854,35 +1759,144 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="36" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="40" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Гиперссылка" xfId="2" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Хороший" xfId="3" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2450,11 +2464,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Q293"/>
+  <dimension ref="A1:S293"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R46" sqref="R46"/>
+      <pane ySplit="7" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S48" sqref="S48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2518,67 +2532,67 @@
     <row r="3" spans="1:17" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="16"/>
-      <c r="C3" s="210"/>
-      <c r="D3" s="211"/>
-      <c r="E3" s="211"/>
-      <c r="F3" s="212" t="s">
+      <c r="C3" s="173"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="174" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="213" t="s">
+      <c r="G3" s="175" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="212" t="s">
+      <c r="H3" s="174" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="213" t="s">
+      <c r="I3" s="175" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="214"/>
-      <c r="K3" s="199"/>
-      <c r="L3" s="199"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
       <c r="M3" s="17"/>
     </row>
     <row r="4" spans="1:17" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="16"/>
-      <c r="C4" s="210"/>
-      <c r="D4" s="211"/>
-      <c r="E4" s="211"/>
-      <c r="F4" s="212" t="s">
+      <c r="C4" s="173"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="174" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="215" t="s">
+      <c r="G4" s="176" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="212" t="s">
+      <c r="H4" s="174" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="214" t="s">
+      <c r="I4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="214"/>
-      <c r="K4" s="199"/>
-      <c r="L4" s="199"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
       <c r="M4" s="17"/>
     </row>
     <row r="5" spans="1:17" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="16"/>
-      <c r="C5" s="210"/>
-      <c r="D5" s="211"/>
-      <c r="E5" s="211"/>
-      <c r="F5" s="212" t="s">
+      <c r="C5" s="173"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="174" t="s">
         <v>0</v>
       </c>
-      <c r="G5" s="216" t="str">
+      <c r="G5" s="177" t="str">
         <f ca="1">MID(CELL("filename"),FIND("[",CELL("filename"))+1, FIND("]",CELL("filename"))-(FIND("[",CELL("filename"))+1))</f>
-        <v>CARRIAGE_BOM.xlsx</v>
-      </c>
-      <c r="H5" s="212"/>
-      <c r="I5" s="196"/>
-      <c r="J5" s="196"/>
-      <c r="K5" s="199"/>
-      <c r="L5" s="199"/>
+        <v>CNC_BOM.xlsx</v>
+      </c>
+      <c r="H5" s="174"/>
+      <c r="I5" s="187"/>
+      <c r="J5" s="187"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
       <c r="M5" s="17"/>
     </row>
     <row r="6" spans="1:17" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -2592,12 +2606,12 @@
       </c>
       <c r="G6" s="22">
         <f ca="1">TODAY()</f>
-        <v>44912</v>
+        <v>44926</v>
       </c>
       <c r="H6" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="217">
+      <c r="I6" s="178">
         <v>1</v>
       </c>
       <c r="J6" s="23"/>
@@ -2607,38 +2621,38 @@
     </row>
     <row r="7" spans="1:17" s="7" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="25"/>
-      <c r="B7" s="200" t="s">
+      <c r="B7" s="165" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="201" t="s">
+      <c r="C7" s="166" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="202" t="s">
+      <c r="D7" s="185" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="203"/>
-      <c r="F7" s="204" t="s">
+      <c r="E7" s="186"/>
+      <c r="F7" s="168" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="205" t="s">
+      <c r="G7" s="169" t="s">
         <v>2</v>
       </c>
-      <c r="H7" s="206" t="s">
+      <c r="H7" s="170" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="207" t="s">
+      <c r="I7" s="167" t="s">
         <v>11</v>
       </c>
-      <c r="J7" s="207" t="s">
+      <c r="J7" s="167" t="s">
         <v>12</v>
       </c>
-      <c r="K7" s="208" t="s">
+      <c r="K7" s="171" t="s">
         <v>29</v>
       </c>
-      <c r="L7" s="198" t="s">
+      <c r="L7" s="164" t="s">
         <v>30</v>
       </c>
-      <c r="M7" s="209" t="s">
+      <c r="M7" s="172" t="s">
         <v>148</v>
       </c>
       <c r="N7" s="26" t="s">
@@ -2653,11 +2667,11 @@
     </row>
     <row r="8" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
-      <c r="B8" s="166" t="s">
+      <c r="B8" s="188" t="s">
         <v>96</v>
       </c>
       <c r="C8" s="28"/>
-      <c r="D8" s="194">
+      <c r="D8" s="191">
         <v>2</v>
       </c>
       <c r="E8" s="29"/>
@@ -2687,9 +2701,9 @@
     </row>
     <row r="9" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
-      <c r="B9" s="167"/>
+      <c r="B9" s="189"/>
       <c r="C9" s="34"/>
-      <c r="D9" s="197"/>
+      <c r="D9" s="192"/>
       <c r="E9" s="35"/>
       <c r="F9" s="36"/>
       <c r="G9" s="37"/>
@@ -2708,9 +2722,9 @@
     </row>
     <row r="10" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
-      <c r="B10" s="193"/>
+      <c r="B10" s="190"/>
       <c r="C10" s="53"/>
-      <c r="D10" s="195"/>
+      <c r="D10" s="193"/>
       <c r="E10" s="104"/>
       <c r="F10" s="127"/>
       <c r="G10" s="127"/>
@@ -2729,13 +2743,13 @@
     </row>
     <row r="11" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
-      <c r="B11" s="168" t="s">
+      <c r="B11" s="179" t="s">
         <v>101</v>
       </c>
-      <c r="C11" s="170" t="s">
+      <c r="C11" s="181" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="178">
+      <c r="D11" s="183">
         <v>1</v>
       </c>
       <c r="E11" s="103"/>
@@ -2765,9 +2779,9 @@
     </row>
     <row r="12" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
-      <c r="B12" s="169"/>
-      <c r="C12" s="171"/>
-      <c r="D12" s="179"/>
+      <c r="B12" s="180"/>
+      <c r="C12" s="182"/>
+      <c r="D12" s="184"/>
       <c r="E12" s="104"/>
       <c r="F12" s="49"/>
       <c r="G12" s="50" t="s">
@@ -2782,11 +2796,11 @@
     </row>
     <row r="13" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
-      <c r="B13" s="166" t="s">
+      <c r="B13" s="188" t="s">
         <v>21</v>
       </c>
       <c r="C13" s="28"/>
-      <c r="D13" s="194">
+      <c r="D13" s="191">
         <v>1</v>
       </c>
       <c r="E13" s="29"/>
@@ -2816,9 +2830,9 @@
     </row>
     <row r="14" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
-      <c r="B14" s="193"/>
+      <c r="B14" s="190"/>
       <c r="C14" s="53"/>
-      <c r="D14" s="195"/>
+      <c r="D14" s="193"/>
       <c r="E14" s="54"/>
       <c r="F14" s="55"/>
       <c r="G14" s="56" t="s">
@@ -2833,11 +2847,11 @@
     </row>
     <row r="15" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
-      <c r="B15" s="187" t="s">
+      <c r="B15" s="194" t="s">
         <v>22</v>
       </c>
       <c r="C15" s="61"/>
-      <c r="D15" s="191">
+      <c r="D15" s="198">
         <v>1</v>
       </c>
       <c r="E15" s="103"/>
@@ -2867,9 +2881,9 @@
     </row>
     <row r="16" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
-      <c r="B16" s="188"/>
+      <c r="B16" s="195"/>
       <c r="C16" s="65"/>
-      <c r="D16" s="192"/>
+      <c r="D16" s="199"/>
       <c r="E16" s="104"/>
       <c r="F16" s="66"/>
       <c r="G16" s="67" t="s">
@@ -3624,13 +3638,13 @@
     </row>
     <row r="38" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
-      <c r="B38" s="187" t="s">
+      <c r="B38" s="194" t="s">
         <v>66</v>
       </c>
-      <c r="C38" s="189" t="s">
+      <c r="C38" s="196" t="s">
         <v>36</v>
       </c>
-      <c r="D38" s="191">
+      <c r="D38" s="198">
         <v>1</v>
       </c>
       <c r="E38" s="103"/>
@@ -3663,9 +3677,9 @@
     </row>
     <row r="39" spans="1:17" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
-      <c r="B39" s="188"/>
-      <c r="C39" s="190"/>
-      <c r="D39" s="192"/>
+      <c r="B39" s="195"/>
+      <c r="C39" s="197"/>
+      <c r="D39" s="199"/>
       <c r="E39" s="104"/>
       <c r="F39" s="51"/>
       <c r="G39" s="50" t="s">
@@ -3726,11 +3740,11 @@
     </row>
     <row r="42" spans="1:17" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
-      <c r="B42" s="166" t="s">
+      <c r="B42" s="188" t="s">
         <v>61</v>
       </c>
-      <c r="C42" s="183"/>
-      <c r="D42" s="176">
+      <c r="C42" s="205"/>
+      <c r="D42" s="200">
         <v>1</v>
       </c>
       <c r="E42" s="29"/>
@@ -3762,9 +3776,9 @@
       <c r="Q42" s="89"/>
     </row>
     <row r="43" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="167"/>
-      <c r="C43" s="184"/>
-      <c r="D43" s="177"/>
+      <c r="B43" s="189"/>
+      <c r="C43" s="206"/>
+      <c r="D43" s="201"/>
       <c r="E43" s="155"/>
       <c r="F43" s="156"/>
       <c r="G43" s="42" t="s">
@@ -3778,11 +3792,11 @@
       <c r="M43" s="44"/>
     </row>
     <row r="44" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="168" t="s">
+      <c r="B44" s="179" t="s">
         <v>63</v>
       </c>
-      <c r="C44" s="170"/>
-      <c r="D44" s="178">
+      <c r="C44" s="181"/>
+      <c r="D44" s="183">
         <v>1</v>
       </c>
       <c r="E44" s="103"/>
@@ -3811,9 +3825,9 @@
       </c>
     </row>
     <row r="45" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="169"/>
-      <c r="C45" s="171"/>
-      <c r="D45" s="179"/>
+      <c r="B45" s="180"/>
+      <c r="C45" s="182"/>
+      <c r="D45" s="184"/>
       <c r="E45" s="104"/>
       <c r="F45" s="131"/>
       <c r="G45" s="132" t="s">
@@ -3827,11 +3841,11 @@
       <c r="M45" s="52"/>
     </row>
     <row r="46" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="174" t="s">
+      <c r="B46" s="213" t="s">
         <v>65</v>
       </c>
-      <c r="C46" s="172"/>
-      <c r="D46" s="176">
+      <c r="C46" s="211"/>
+      <c r="D46" s="200">
         <v>2</v>
       </c>
       <c r="E46" s="29"/>
@@ -3860,9 +3874,9 @@
       </c>
     </row>
     <row r="47" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="175"/>
-      <c r="C47" s="173"/>
-      <c r="D47" s="180"/>
+      <c r="B47" s="214"/>
+      <c r="C47" s="212"/>
+      <c r="D47" s="202"/>
       <c r="E47" s="54"/>
       <c r="F47" s="120"/>
       <c r="G47" s="127" t="s">
@@ -3876,11 +3890,11 @@
       <c r="M47" s="60"/>
     </row>
     <row r="48" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B48" s="164" t="s">
+      <c r="B48" s="209" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="185"/>
-      <c r="D48" s="181">
+      <c r="C48" s="207"/>
+      <c r="D48" s="203">
         <v>1</v>
       </c>
       <c r="E48" s="135"/>
@@ -3908,10 +3922,10 @@
         <v>1.21</v>
       </c>
     </row>
-    <row r="49" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="165"/>
-      <c r="C49" s="186"/>
-      <c r="D49" s="182"/>
+    <row r="49" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="210"/>
+      <c r="C49" s="208"/>
+      <c r="D49" s="204"/>
       <c r="E49" s="139"/>
       <c r="F49" s="140"/>
       <c r="G49" s="141" t="s">
@@ -3924,7 +3938,7 @@
       <c r="L49" s="143"/>
       <c r="M49" s="52"/>
     </row>
-    <row r="50" spans="2:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="K50" s="160" t="s">
         <v>149</v>
       </c>
@@ -3934,7 +3948,7 @@
         <v>194.13000000000002</v>
       </c>
     </row>
-    <row r="51" spans="2:13" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:19" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B51" s="94" t="s">
         <v>10</v>
       </c>
@@ -3948,7 +3962,7 @@
       <c r="J51" s="95"/>
       <c r="K51" s="96"/>
     </row>
-    <row r="52" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B52" s="70" t="s">
         <v>66</v>
       </c>
@@ -3981,7 +3995,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="53" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B53" s="112" t="s">
         <v>66</v>
       </c>
@@ -4014,7 +4028,7 @@
         <v>3.9000000000000004</v>
       </c>
     </row>
-    <row r="54" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B54" s="70" t="s">
         <v>66</v>
       </c>
@@ -4047,7 +4061,7 @@
         <v>5.16</v>
       </c>
     </row>
-    <row r="55" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B55" s="112" t="s">
         <v>66</v>
       </c>
@@ -4080,7 +4094,7 @@
         <v>35.200000000000003</v>
       </c>
     </row>
-    <row r="56" spans="2:13" ht="15" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:19" ht="15" x14ac:dyDescent="0.2">
       <c r="B56" s="98" t="s">
         <v>66</v>
       </c>
@@ -4113,7 +4127,7 @@
         <v>21.78</v>
       </c>
     </row>
-    <row r="57" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B57" s="118"/>
       <c r="C57" s="119"/>
       <c r="D57" s="54"/>
@@ -4133,7 +4147,7 @@
       <c r="L57" s="149"/>
       <c r="M57" s="60"/>
     </row>
-    <row r="58" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B58" s="112" t="s">
         <v>66</v>
       </c>
@@ -4166,7 +4180,7 @@
         <v>2.92</v>
       </c>
     </row>
-    <row r="59" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B59" s="70" t="s">
         <v>66</v>
       </c>
@@ -4199,7 +4213,7 @@
         <v>3.1619999999999999</v>
       </c>
     </row>
-    <row r="60" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B60" s="112" t="s">
         <v>66</v>
       </c>
@@ -4232,7 +4246,7 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="61" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B61" s="70" t="s">
         <v>66</v>
       </c>
@@ -4265,13 +4279,13 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="62" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B62" s="112" t="s">
         <v>66</v>
       </c>
       <c r="C62" s="113"/>
       <c r="D62" s="114">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E62" s="114"/>
       <c r="F62" s="115"/>
@@ -4285,9 +4299,9 @@
         <v>31</v>
       </c>
       <c r="J62" s="115" t="s">
-        <v>69</v>
-      </c>
-      <c r="K62" s="117" t="s">
+        <v>153</v>
+      </c>
+      <c r="K62" s="216" t="s">
         <v>31</v>
       </c>
       <c r="L62" s="159">
@@ -4295,10 +4309,11 @@
       </c>
       <c r="M62" s="81">
         <f t="shared" si="2"/>
-        <v>7.48</v>
-      </c>
-    </row>
-    <row r="63" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>7.04</v>
+      </c>
+      <c r="S62" s="215"/>
+    </row>
+    <row r="63" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B63" s="70" t="s">
         <v>66</v>
       </c>
@@ -4331,13 +4346,13 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="64" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B64" s="112" t="s">
         <v>66</v>
       </c>
       <c r="C64" s="113"/>
       <c r="D64" s="114">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E64" s="114"/>
       <c r="F64" s="115"/>
@@ -4361,8 +4376,9 @@
       </c>
       <c r="M64" s="81">
         <f t="shared" si="2"/>
-        <v>0.84</v>
-      </c>
+        <v>0.48</v>
+      </c>
+      <c r="S64" s="215"/>
     </row>
     <row r="65" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B65" s="70" t="s">
@@ -4638,7 +4654,7 @@
       <c r="L73" s="161"/>
       <c r="M73" s="162">
         <f>SUM(M52:M72)</f>
-        <v>140.24200000000002</v>
+        <v>139.44200000000001</v>
       </c>
     </row>
     <row r="74" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -4654,7 +4670,7 @@
       <c r="L75" s="161"/>
       <c r="M75" s="162">
         <f>M40+M50+M73</f>
-        <v>1756.5519999999999</v>
+        <v>1755.752</v>
       </c>
     </row>
     <row r="76" spans="2:13" x14ac:dyDescent="0.2">
@@ -5531,6 +5547,25 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="D15:D16"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:D12"/>
@@ -5538,25 +5573,6 @@
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="D8:D10"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="B46:B47"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
updated drawings, some little changes
</commit_message>
<xml_diff>
--- a/Drawings/CNC_BOM.xlsx
+++ b/Drawings/CNC_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\development\GitHub\LaserCNCMachine\Drawings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3743860E-75AD-41D0-9C4F-962EC7D48465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83578765-F4EF-4C94-BDA7-2305B64F46FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="150">
   <si>
     <t>File</t>
   </si>
@@ -131,9 +131,6 @@
     <t>2</t>
   </si>
   <si>
-    <t>Corner Bracket 40х40L</t>
-  </si>
-  <si>
     <t>AISI 1035 Steel (SS)</t>
   </si>
   <si>
@@ -141,9 +138,6 @@
   </si>
   <si>
     <t>M5 NYLOC DIN 985</t>
-  </si>
-  <si>
-    <t>M4 NYLOC DIN 985</t>
   </si>
   <si>
     <t>Washer DIN 125 - A 5.3</t>
@@ -527,6 +521,24 @@
   </si>
   <si>
     <t>ISO 10642 - M3 x 16 - 16N</t>
+  </si>
+  <si>
+    <t>500214</t>
+  </si>
+  <si>
+    <t>5100214</t>
+  </si>
+  <si>
+    <t>T nut 2020 М5</t>
+  </si>
+  <si>
+    <t>написать сюда аналог!</t>
+  </si>
+  <si>
+    <t>Corner Bracket 40х20L</t>
+  </si>
+  <si>
+    <t>добавить аналог</t>
   </si>
 </sst>
 </file>
@@ -1687,85 +1699,85 @@
     <xf numFmtId="49" fontId="9" fillId="0" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="36" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="40" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="36" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="40" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -2339,11 +2351,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:S290"/>
+  <dimension ref="A1:T290"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R50" sqref="R50"/>
+      <pane ySplit="7" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2392,7 +2404,7 @@
         <v>8</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H2" s="11" t="s">
         <v>15</v>
@@ -2415,13 +2427,13 @@
         <v>6</v>
       </c>
       <c r="G3" s="163" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H3" s="162" t="s">
         <v>17</v>
       </c>
       <c r="I3" s="163" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="J3" s="5"/>
       <c r="K3" s="1"/>
@@ -2462,11 +2474,11 @@
       </c>
       <c r="G5" s="165" t="str">
         <f ca="1">MID(CELL("filename"),FIND("[",CELL("filename"))+1, FIND("]",CELL("filename"))-(FIND("[",CELL("filename"))+1))</f>
-        <v>CNC.xlsx</v>
+        <v>CNC_BOM.xlsx</v>
       </c>
       <c r="H5" s="162"/>
-      <c r="I5" s="192"/>
-      <c r="J5" s="192"/>
+      <c r="I5" s="179"/>
+      <c r="J5" s="179"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="17"/>
@@ -2482,7 +2494,7 @@
       </c>
       <c r="G6" s="22">
         <f ca="1">TODAY()</f>
-        <v>44940</v>
+        <v>44941</v>
       </c>
       <c r="H6" s="21" t="s">
         <v>5</v>
@@ -2503,10 +2515,10 @@
       <c r="C7" s="154" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="190" t="s">
+      <c r="D7" s="177" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="191"/>
+      <c r="E7" s="178"/>
       <c r="F7" s="156" t="s">
         <v>4</v>
       </c>
@@ -2529,7 +2541,7 @@
         <v>27</v>
       </c>
       <c r="M7" s="160" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N7" s="26" t="s">
         <v>30</v>
@@ -2543,26 +2555,26 @@
     </row>
     <row r="8" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
-      <c r="B8" s="169" t="s">
-        <v>76</v>
+      <c r="B8" s="180" t="s">
+        <v>74</v>
       </c>
       <c r="C8" s="28"/>
-      <c r="D8" s="188">
+      <c r="D8" s="183">
         <v>2</v>
       </c>
       <c r="E8" s="29"/>
       <c r="F8" s="30"/>
       <c r="G8" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="H8" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="H8" s="29" t="s">
-        <v>77</v>
-      </c>
       <c r="I8" s="31" t="s">
         <v>28</v>
       </c>
       <c r="J8" s="31" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K8" s="32" t="s">
         <v>28</v>
@@ -2577,9 +2589,9 @@
     </row>
     <row r="9" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
-      <c r="B9" s="170"/>
+      <c r="B9" s="181"/>
       <c r="C9" s="34"/>
-      <c r="D9" s="193"/>
+      <c r="D9" s="184"/>
       <c r="E9" s="35"/>
       <c r="F9" s="36"/>
       <c r="G9" s="37"/>
@@ -2588,7 +2600,7 @@
         <v>28</v>
       </c>
       <c r="J9" s="39" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K9" s="40" t="s">
         <v>28</v>
@@ -2598,21 +2610,21 @@
     </row>
     <row r="10" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
-      <c r="B10" s="187"/>
+      <c r="B10" s="182"/>
       <c r="C10" s="53"/>
-      <c r="D10" s="189"/>
+      <c r="D10" s="185"/>
       <c r="E10" s="104"/>
       <c r="F10" s="127"/>
       <c r="G10" s="127"/>
       <c r="H10" s="127"/>
       <c r="I10" s="58" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J10" s="58" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K10" s="141" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L10" s="137"/>
       <c r="M10" s="60"/>
@@ -2620,30 +2632,30 @@
     <row r="11" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="171" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C11" s="173" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="177">
+      <c r="D11" s="175">
         <v>1</v>
       </c>
       <c r="E11" s="103"/>
       <c r="F11" s="45"/>
       <c r="G11" s="46" t="s">
+        <v>78</v>
+      </c>
+      <c r="H11" s="103" t="s">
         <v>80</v>
       </c>
-      <c r="H11" s="103" t="s">
-        <v>82</v>
-      </c>
       <c r="I11" s="46" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J11" s="46" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K11" s="47" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L11" s="135">
         <v>62.17</v>
@@ -2657,11 +2669,11 @@
       <c r="A12" s="3"/>
       <c r="B12" s="172"/>
       <c r="C12" s="174"/>
-      <c r="D12" s="178"/>
+      <c r="D12" s="176"/>
       <c r="E12" s="104"/>
       <c r="F12" s="49"/>
       <c r="G12" s="50" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H12" s="51"/>
       <c r="I12" s="51"/>
@@ -2672,11 +2684,11 @@
     </row>
     <row r="13" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
-      <c r="B13" s="169" t="s">
+      <c r="B13" s="180" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="28"/>
-      <c r="D13" s="188">
+      <c r="D13" s="183">
         <v>1</v>
       </c>
       <c r="E13" s="29"/>
@@ -2685,7 +2697,7 @@
         <v>21</v>
       </c>
       <c r="H13" s="29" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I13" s="31" t="s">
         <v>28</v>
@@ -2706,13 +2718,13 @@
     </row>
     <row r="14" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
-      <c r="B14" s="187"/>
+      <c r="B14" s="182"/>
       <c r="C14" s="53"/>
-      <c r="D14" s="189"/>
+      <c r="D14" s="185"/>
       <c r="E14" s="54"/>
       <c r="F14" s="55"/>
       <c r="G14" s="56" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H14" s="57"/>
       <c r="I14" s="58"/>
@@ -2723,11 +2735,11 @@
     </row>
     <row r="15" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
-      <c r="B15" s="181" t="s">
+      <c r="B15" s="186" t="s">
         <v>19</v>
       </c>
       <c r="C15" s="61"/>
-      <c r="D15" s="185">
+      <c r="D15" s="190">
         <v>1</v>
       </c>
       <c r="E15" s="103"/>
@@ -2736,7 +2748,7 @@
         <v>22</v>
       </c>
       <c r="H15" s="103" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I15" s="46" t="s">
         <v>28</v>
@@ -2757,13 +2769,13 @@
     </row>
     <row r="16" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
-      <c r="B16" s="182"/>
+      <c r="B16" s="187"/>
       <c r="C16" s="65"/>
-      <c r="D16" s="186"/>
+      <c r="D16" s="191"/>
       <c r="E16" s="104"/>
       <c r="F16" s="66"/>
       <c r="G16" s="67" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H16" s="68"/>
       <c r="I16" s="51"/>
@@ -2772,10 +2784,10 @@
       <c r="L16" s="136"/>
       <c r="M16" s="52"/>
     </row>
-    <row r="17" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="70" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C17" s="71"/>
       <c r="D17" s="72">
@@ -2784,16 +2796,16 @@
       <c r="E17" s="72"/>
       <c r="F17" s="73"/>
       <c r="G17" s="74" t="s">
+        <v>82</v>
+      </c>
+      <c r="H17" s="72" t="s">
+        <v>34</v>
+      </c>
+      <c r="I17" s="74" t="s">
+        <v>28</v>
+      </c>
+      <c r="J17" s="74" t="s">
         <v>84</v>
-      </c>
-      <c r="H17" s="72" t="s">
-        <v>35</v>
-      </c>
-      <c r="I17" s="74" t="s">
-        <v>28</v>
-      </c>
-      <c r="J17" s="74" t="s">
-        <v>86</v>
       </c>
       <c r="K17" s="106" t="s">
         <v>28</v>
@@ -2806,10 +2818,10 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="76" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C18" s="77"/>
       <c r="D18" s="78">
@@ -2818,16 +2830,16 @@
       <c r="E18" s="78"/>
       <c r="F18" s="79"/>
       <c r="G18" s="80" t="s">
+        <v>86</v>
+      </c>
+      <c r="H18" s="78" t="s">
+        <v>87</v>
+      </c>
+      <c r="I18" s="80" t="s">
+        <v>28</v>
+      </c>
+      <c r="J18" s="80" t="s">
         <v>88</v>
-      </c>
-      <c r="H18" s="78" t="s">
-        <v>89</v>
-      </c>
-      <c r="I18" s="80" t="s">
-        <v>28</v>
-      </c>
-      <c r="J18" s="80" t="s">
-        <v>90</v>
       </c>
       <c r="K18" s="142" t="s">
         <v>28</v>
@@ -2840,10 +2852,10 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="70" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C19" s="71"/>
       <c r="D19" s="72">
@@ -2852,19 +2864,19 @@
       <c r="E19" s="72"/>
       <c r="F19" s="73"/>
       <c r="G19" s="74" t="s">
+        <v>89</v>
+      </c>
+      <c r="H19" s="72" t="s">
         <v>91</v>
       </c>
-      <c r="H19" s="72" t="s">
-        <v>93</v>
-      </c>
       <c r="I19" s="74" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J19" s="74" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K19" s="82" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L19" s="138">
         <v>0.48</v>
@@ -2875,10 +2887,10 @@
       </c>
       <c r="O19" s="83"/>
     </row>
-    <row r="20" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="76" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C20" s="77"/>
       <c r="D20" s="78">
@@ -2887,16 +2899,16 @@
       <c r="E20" s="78"/>
       <c r="F20" s="79"/>
       <c r="G20" s="80" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H20" s="78" t="s">
+        <v>91</v>
+      </c>
+      <c r="I20" s="80" t="s">
+        <v>28</v>
+      </c>
+      <c r="J20" s="80" t="s">
         <v>93</v>
-      </c>
-      <c r="I20" s="80" t="s">
-        <v>28</v>
-      </c>
-      <c r="J20" s="80" t="s">
-        <v>95</v>
       </c>
       <c r="K20" s="142" t="s">
         <v>28</v>
@@ -2909,10 +2921,10 @@
         <v>4.38</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="70" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C21" s="71"/>
       <c r="D21" s="72">
@@ -2921,19 +2933,19 @@
       <c r="E21" s="72"/>
       <c r="F21" s="73"/>
       <c r="G21" s="74" t="s">
+        <v>148</v>
+      </c>
+      <c r="H21" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="H21" s="72" t="s">
-        <v>35</v>
-      </c>
       <c r="I21" s="74" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J21" s="74" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K21" s="106" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="L21" s="138">
         <v>49</v>
@@ -2942,11 +2954,12 @@
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" s="86" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S21" s="167"/>
+    </row>
+    <row r="22" spans="1:20" s="86" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="84"/>
       <c r="B22" s="76" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C22" s="77"/>
       <c r="D22" s="78">
@@ -2955,19 +2968,19 @@
       <c r="E22" s="78"/>
       <c r="F22" s="79"/>
       <c r="G22" s="80" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H22" s="78" t="s">
         <v>24</v>
       </c>
       <c r="I22" s="80" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J22" s="80" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K22" s="85" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L22" s="140">
         <v>25</v>
@@ -2977,10 +2990,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="86" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" s="86" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="84"/>
       <c r="B23" s="70" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C23" s="71"/>
       <c r="D23" s="72">
@@ -2989,19 +3002,19 @@
       <c r="E23" s="72"/>
       <c r="F23" s="73"/>
       <c r="G23" s="74" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H23" s="72" t="s">
         <v>24</v>
       </c>
       <c r="I23" s="74" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J23" s="74" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K23" s="82" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L23" s="138">
         <v>37</v>
@@ -3011,44 +3024,48 @@
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="76" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C24" s="77"/>
       <c r="D24" s="78">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E24" s="78"/>
       <c r="F24" s="79"/>
       <c r="G24" s="80" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H24" s="78" t="s">
         <v>24</v>
       </c>
       <c r="I24" s="80" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J24" s="80" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K24" s="85" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L24" s="140">
         <v>1.6</v>
       </c>
       <c r="M24" s="81">
         <f t="shared" si="0"/>
-        <v>3.2</v>
+        <v>6.4</v>
       </c>
       <c r="O24" s="83"/>
-    </row>
-    <row r="25" spans="1:17" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S24" s="167"/>
+      <c r="T24" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="87"/>
       <c r="B25" s="70" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C25" s="71"/>
       <c r="D25" s="72">
@@ -3057,19 +3074,19 @@
       <c r="E25" s="72"/>
       <c r="F25" s="73"/>
       <c r="G25" s="74" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H25" s="72" t="s">
         <v>24</v>
       </c>
       <c r="I25" s="74" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J25" s="74" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K25" s="82" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L25" s="138">
         <v>315</v>
@@ -3082,10 +3099,10 @@
       <c r="O25" s="88"/>
       <c r="Q25" s="89"/>
     </row>
-    <row r="26" spans="1:17" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="87"/>
       <c r="B26" s="76" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C26" s="77"/>
       <c r="D26" s="78">
@@ -3094,16 +3111,16 @@
       <c r="E26" s="78"/>
       <c r="F26" s="79"/>
       <c r="G26" s="80" t="s">
+        <v>96</v>
+      </c>
+      <c r="H26" s="78" t="s">
+        <v>97</v>
+      </c>
+      <c r="I26" s="80" t="s">
+        <v>28</v>
+      </c>
+      <c r="J26" s="80" t="s">
         <v>98</v>
-      </c>
-      <c r="H26" s="78" t="s">
-        <v>99</v>
-      </c>
-      <c r="I26" s="80" t="s">
-        <v>28</v>
-      </c>
-      <c r="J26" s="80" t="s">
-        <v>100</v>
       </c>
       <c r="K26" s="142" t="s">
         <v>28</v>
@@ -3119,10 +3136,10 @@
       <c r="O26" s="88"/>
       <c r="Q26" s="89"/>
     </row>
-    <row r="27" spans="1:17" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="87"/>
       <c r="B27" s="70" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C27" s="71"/>
       <c r="D27" s="72">
@@ -3131,19 +3148,19 @@
       <c r="E27" s="72"/>
       <c r="F27" s="73"/>
       <c r="G27" s="74" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H27" s="72" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I27" s="74" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J27" s="74" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K27" s="82" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L27" s="138">
         <v>1.34</v>
@@ -3156,9 +3173,9 @@
       <c r="O27" s="88"/>
       <c r="Q27" s="89"/>
     </row>
-    <row r="28" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B28" s="76" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C28" s="77"/>
       <c r="D28" s="78">
@@ -3167,16 +3184,16 @@
       <c r="E28" s="78"/>
       <c r="F28" s="79"/>
       <c r="G28" s="80" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H28" s="78" t="s">
+        <v>100</v>
+      </c>
+      <c r="I28" s="80" t="s">
+        <v>28</v>
+      </c>
+      <c r="J28" s="80" t="s">
         <v>102</v>
-      </c>
-      <c r="I28" s="80" t="s">
-        <v>28</v>
-      </c>
-      <c r="J28" s="80" t="s">
-        <v>104</v>
       </c>
       <c r="K28" s="142" t="s">
         <v>28</v>
@@ -3189,9 +3206,9 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B29" s="70" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C29" s="71"/>
       <c r="D29" s="72">
@@ -3200,16 +3217,16 @@
       <c r="E29" s="72"/>
       <c r="F29" s="73"/>
       <c r="G29" s="74" t="s">
+        <v>103</v>
+      </c>
+      <c r="H29" s="72" t="s">
+        <v>104</v>
+      </c>
+      <c r="I29" s="74" t="s">
+        <v>28</v>
+      </c>
+      <c r="J29" s="74" t="s">
         <v>105</v>
-      </c>
-      <c r="H29" s="72" t="s">
-        <v>106</v>
-      </c>
-      <c r="I29" s="74" t="s">
-        <v>28</v>
-      </c>
-      <c r="J29" s="74" t="s">
-        <v>107</v>
       </c>
       <c r="K29" s="106" t="s">
         <v>28</v>
@@ -3222,10 +3239,10 @@
         <v>7.93</v>
       </c>
     </row>
-    <row r="30" spans="1:17" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="87"/>
       <c r="B30" s="76" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C30" s="77"/>
       <c r="D30" s="78">
@@ -3234,19 +3251,19 @@
       <c r="E30" s="78"/>
       <c r="F30" s="79"/>
       <c r="G30" s="80" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H30" s="78" t="s">
         <v>24</v>
       </c>
       <c r="I30" s="80" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J30" s="80" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K30" s="85" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L30" s="140">
         <v>314</v>
@@ -3259,9 +3276,9 @@
       <c r="O30" s="88"/>
       <c r="Q30" s="89"/>
     </row>
-    <row r="31" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B31" s="70" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C31" s="71"/>
       <c r="D31" s="72">
@@ -3270,19 +3287,19 @@
       <c r="E31" s="72"/>
       <c r="F31" s="73"/>
       <c r="G31" s="74" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H31" s="72" t="s">
         <v>24</v>
       </c>
       <c r="I31" s="74" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J31" s="74" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K31" s="82" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L31" s="138">
         <v>5.1100000000000003</v>
@@ -3292,10 +3309,10 @@
         <v>10.220000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:17" s="91" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" s="91" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="90"/>
       <c r="B32" s="76" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C32" s="77"/>
       <c r="D32" s="78">
@@ -3304,19 +3321,19 @@
       <c r="E32" s="78"/>
       <c r="F32" s="79"/>
       <c r="G32" s="80" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H32" s="78" t="s">
         <v>24</v>
       </c>
       <c r="I32" s="80" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J32" s="80" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K32" s="85" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L32" s="140">
         <v>49</v>
@@ -3330,7 +3347,7 @@
     <row r="33" spans="1:18" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="84"/>
       <c r="B33" s="70" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C33" s="71"/>
       <c r="D33" s="72">
@@ -3339,19 +3356,19 @@
       <c r="E33" s="72"/>
       <c r="F33" s="73"/>
       <c r="G33" s="74" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H33" s="72" t="s">
         <v>24</v>
       </c>
       <c r="I33" s="74" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J33" s="74" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K33" s="82" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L33" s="138">
         <v>10</v>
@@ -3367,7 +3384,7 @@
     <row r="34" spans="1:18" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="76" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C34" s="77"/>
       <c r="D34" s="78">
@@ -3376,19 +3393,19 @@
       <c r="E34" s="78"/>
       <c r="F34" s="79"/>
       <c r="G34" s="80" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H34" s="78" t="s">
         <v>24</v>
       </c>
       <c r="I34" s="80" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J34" s="80" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K34" s="85" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L34" s="140">
         <v>16</v>
@@ -3404,7 +3421,7 @@
     <row r="35" spans="1:18" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="90"/>
       <c r="B35" s="70" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C35" s="71"/>
       <c r="D35" s="72">
@@ -3413,7 +3430,7 @@
       <c r="E35" s="72"/>
       <c r="F35" s="73"/>
       <c r="G35" s="74" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H35" s="72" t="s">
         <v>24</v>
@@ -3422,7 +3439,7 @@
         <v>28</v>
       </c>
       <c r="J35" s="74" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K35" s="106" t="s">
         <v>28</v>
@@ -3441,7 +3458,7 @@
     <row r="36" spans="1:18" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="76" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C36" s="77"/>
       <c r="D36" s="78">
@@ -3450,7 +3467,7 @@
       <c r="E36" s="78"/>
       <c r="F36" s="79"/>
       <c r="G36" s="80" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H36" s="78" t="s">
         <v>24</v>
@@ -3459,7 +3476,7 @@
         <v>28</v>
       </c>
       <c r="J36" s="80" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K36" s="142" t="s">
         <v>28</v>
@@ -3478,7 +3495,7 @@
     <row r="37" spans="1:18" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="87"/>
       <c r="B37" s="70" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C37" s="71"/>
       <c r="D37" s="72">
@@ -3487,19 +3504,19 @@
       <c r="E37" s="72"/>
       <c r="F37" s="73"/>
       <c r="G37" s="74" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H37" s="72" t="s">
         <v>24</v>
       </c>
       <c r="I37" s="74" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="J37" s="74" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K37" s="82" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="L37" s="138">
         <v>1</v>
@@ -3514,31 +3531,31 @@
     </row>
     <row r="38" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
-      <c r="B38" s="181" t="s">
-        <v>55</v>
-      </c>
-      <c r="C38" s="183" t="s">
+      <c r="B38" s="186" t="s">
+        <v>53</v>
+      </c>
+      <c r="C38" s="188" t="s">
         <v>33</v>
       </c>
-      <c r="D38" s="185">
+      <c r="D38" s="190">
         <v>1</v>
       </c>
       <c r="E38" s="103"/>
       <c r="F38" s="62"/>
       <c r="G38" s="46" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H38" s="103" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I38" s="46" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J38" s="46" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K38" s="47" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L38" s="135">
         <v>11.5</v>
@@ -3553,13 +3570,13 @@
     </row>
     <row r="39" spans="1:18" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
-      <c r="B39" s="182"/>
-      <c r="C39" s="184"/>
-      <c r="D39" s="186"/>
+      <c r="B39" s="187"/>
+      <c r="C39" s="189"/>
+      <c r="D39" s="191"/>
       <c r="E39" s="104"/>
       <c r="F39" s="51"/>
       <c r="G39" s="50" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H39" s="104"/>
       <c r="I39" s="51"/>
@@ -3583,12 +3600,12 @@
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
       <c r="K40" s="148" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="L40" s="151"/>
       <c r="M40" s="150">
         <f>SUM(M8:M39)</f>
-        <v>1422.1799999999998</v>
+        <v>1425.3799999999999</v>
       </c>
       <c r="N40" s="1"/>
       <c r="O40" s="88"/>
@@ -3597,7 +3614,7 @@
     <row r="41" spans="1:18" s="5" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="107" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="3"/>
@@ -3616,26 +3633,26 @@
     </row>
     <row r="42" spans="1:18" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
-      <c r="B42" s="169" t="s">
-        <v>132</v>
-      </c>
-      <c r="C42" s="179"/>
-      <c r="D42" s="175">
+      <c r="B42" s="180" t="s">
+        <v>130</v>
+      </c>
+      <c r="C42" s="194"/>
+      <c r="D42" s="192">
         <v>1</v>
       </c>
       <c r="E42" s="29"/>
       <c r="F42" s="126"/>
       <c r="G42" s="31" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H42" s="29" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I42" s="31" t="s">
         <v>28</v>
       </c>
       <c r="J42" s="31" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K42" s="102" t="s">
         <v>28</v>
@@ -3650,16 +3667,16 @@
       <c r="N42" s="1"/>
       <c r="O42" s="88"/>
       <c r="Q42" s="89"/>
-      <c r="R42" s="194"/>
+      <c r="R42" s="169"/>
     </row>
     <row r="43" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="170"/>
-      <c r="C43" s="180"/>
-      <c r="D43" s="176"/>
+      <c r="B43" s="181"/>
+      <c r="C43" s="195"/>
+      <c r="D43" s="193"/>
       <c r="E43" s="143"/>
       <c r="F43" s="144"/>
       <c r="G43" s="42" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H43" s="145"/>
       <c r="I43" s="43"/>
@@ -3670,25 +3687,25 @@
     </row>
     <row r="44" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="171" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C44" s="173"/>
-      <c r="D44" s="177">
+      <c r="D44" s="175">
         <v>2</v>
       </c>
       <c r="E44" s="103"/>
       <c r="F44" s="128"/>
       <c r="G44" s="46" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H44" s="103" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I44" s="46" t="s">
         <v>28</v>
       </c>
       <c r="J44" s="46" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K44" s="129" t="s">
         <v>28</v>
@@ -3705,11 +3722,11 @@
     <row r="45" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B45" s="172"/>
       <c r="C45" s="174"/>
-      <c r="D45" s="178"/>
+      <c r="D45" s="176"/>
       <c r="E45" s="104"/>
       <c r="F45" s="130"/>
       <c r="G45" s="131" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H45" s="68"/>
       <c r="I45" s="51"/>
@@ -3720,7 +3737,7 @@
     </row>
     <row r="46" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="K46" s="148" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="L46" s="149"/>
       <c r="M46" s="150">
@@ -3744,7 +3761,7 @@
     </row>
     <row r="48" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B48" s="70" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C48" s="108"/>
       <c r="D48" s="72">
@@ -3753,19 +3770,19 @@
       <c r="E48" s="72"/>
       <c r="F48" s="109"/>
       <c r="G48" s="109" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H48" s="110" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I48" s="109" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J48" s="109" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K48" s="111" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L48" s="138">
         <v>0.23</v>
@@ -3775,42 +3792,43 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="49" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B49" s="112" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C49" s="113"/>
       <c r="D49" s="114">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="E49" s="114"/>
       <c r="F49" s="115"/>
       <c r="G49" s="115" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H49" s="116" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I49" s="115" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J49" s="115" t="s">
-        <v>57</v>
+        <v>144</v>
       </c>
       <c r="K49" s="117" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L49" s="147">
-        <v>0.65</v>
+        <v>0.4</v>
       </c>
       <c r="M49" s="81">
         <f t="shared" si="2"/>
-        <v>3.9000000000000004</v>
-      </c>
-    </row>
-    <row r="50" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>22.400000000000002</v>
+      </c>
+      <c r="S49" s="167"/>
+    </row>
+    <row r="50" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B50" s="70" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C50" s="108"/>
       <c r="D50" s="72">
@@ -3819,64 +3837,66 @@
       <c r="E50" s="72"/>
       <c r="F50" s="109"/>
       <c r="G50" s="109" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="H50" s="110" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I50" s="109" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="J50" s="109" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K50" s="111" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="L50" s="138">
-        <v>1.29</v>
+        <v>5.27</v>
       </c>
       <c r="M50" s="75">
         <f t="shared" si="2"/>
-        <v>5.16</v>
-      </c>
-    </row>
-    <row r="51" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>21.08</v>
+      </c>
+      <c r="S50" s="167"/>
+    </row>
+    <row r="51" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B51" s="112" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C51" s="113"/>
       <c r="D51" s="114">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E51" s="114"/>
       <c r="F51" s="115"/>
       <c r="G51" s="115" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H51" s="116" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I51" s="115" t="s">
         <v>28</v>
       </c>
       <c r="J51" s="115" t="s">
-        <v>57</v>
+        <v>145</v>
       </c>
       <c r="K51" s="117" t="s">
         <v>28</v>
       </c>
       <c r="L51" s="147">
-        <v>1.6</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="M51" s="81">
         <f t="shared" si="2"/>
-        <v>35.200000000000003</v>
-      </c>
-    </row>
-    <row r="52" spans="2:19" ht="15" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+      <c r="S51" s="167"/>
+    </row>
+    <row r="52" spans="2:20" ht="15" x14ac:dyDescent="0.2">
       <c r="B52" s="98" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C52" s="99"/>
       <c r="D52" s="29">
@@ -3885,19 +3905,19 @@
       <c r="E52" s="29"/>
       <c r="F52" s="100"/>
       <c r="G52" s="100" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H52" s="101" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I52" s="100" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J52" s="100" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K52" s="102" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L52" s="133">
         <v>3.63</v>
@@ -3907,7 +3927,7 @@
         <v>21.78</v>
       </c>
     </row>
-    <row r="53" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B53" s="118"/>
       <c r="C53" s="119"/>
       <c r="D53" s="54"/>
@@ -3919,7 +3939,7 @@
         <v>28</v>
       </c>
       <c r="J53" s="120" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K53" s="121" t="s">
         <v>28</v>
@@ -3927,9 +3947,9 @@
       <c r="L53" s="137"/>
       <c r="M53" s="60"/>
     </row>
-    <row r="54" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B54" s="112" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C54" s="113"/>
       <c r="D54" s="114">
@@ -3938,16 +3958,16 @@
       <c r="E54" s="114"/>
       <c r="F54" s="115"/>
       <c r="G54" s="115" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H54" s="116" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I54" s="115" t="s">
         <v>28</v>
       </c>
       <c r="J54" s="115" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K54" s="117" t="s">
         <v>28</v>
@@ -3960,9 +3980,9 @@
         <v>2.92</v>
       </c>
     </row>
-    <row r="55" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B55" s="70" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C55" s="108"/>
       <c r="D55" s="72">
@@ -3971,16 +3991,16 @@
       <c r="E55" s="72"/>
       <c r="F55" s="109"/>
       <c r="G55" s="109" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H55" s="110" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I55" s="109" t="s">
         <v>28</v>
       </c>
       <c r="J55" s="109" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K55" s="111" t="s">
         <v>28</v>
@@ -3993,9 +4013,9 @@
         <v>3.1619999999999999</v>
       </c>
     </row>
-    <row r="56" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B56" s="112" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C56" s="113"/>
       <c r="D56" s="114">
@@ -4004,16 +4024,16 @@
       <c r="E56" s="114"/>
       <c r="F56" s="115"/>
       <c r="G56" s="115" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H56" s="116" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I56" s="115" t="s">
         <v>28</v>
       </c>
       <c r="J56" s="115" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K56" s="117" t="s">
         <v>28</v>
@@ -4027,9 +4047,9 @@
       </c>
       <c r="S56" s="167"/>
     </row>
-    <row r="57" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B57" s="70" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C57" s="108"/>
       <c r="D57" s="72">
@@ -4038,16 +4058,16 @@
       <c r="E57" s="72"/>
       <c r="F57" s="109"/>
       <c r="G57" s="109" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H57" s="110" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I57" s="109" t="s">
         <v>28</v>
       </c>
       <c r="J57" s="109" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K57" s="111" t="s">
         <v>28</v>
@@ -4060,9 +4080,9 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="58" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B58" s="112" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C58" s="113"/>
       <c r="D58" s="114">
@@ -4071,16 +4091,16 @@
       <c r="E58" s="114"/>
       <c r="F58" s="115"/>
       <c r="G58" s="115" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H58" s="116" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I58" s="115" t="s">
         <v>28</v>
       </c>
       <c r="J58" s="115" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="K58" s="168" t="s">
         <v>28</v>
@@ -4094,23 +4114,46 @@
       </c>
       <c r="S58" s="167"/>
     </row>
-    <row r="59" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="70"/>
+    <row r="59" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="70" t="s">
+        <v>53</v>
+      </c>
       <c r="C59" s="108"/>
-      <c r="D59" s="72"/>
+      <c r="D59" s="72">
+        <v>32</v>
+      </c>
       <c r="E59" s="72"/>
       <c r="F59" s="109"/>
-      <c r="G59" s="109"/>
-      <c r="H59" s="110"/>
-      <c r="I59" s="109"/>
-      <c r="J59" s="109"/>
-      <c r="K59" s="111"/>
-      <c r="L59" s="138"/>
-      <c r="M59" s="75"/>
-    </row>
-    <row r="60" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G59" s="109" t="s">
+        <v>146</v>
+      </c>
+      <c r="H59" s="110" t="s">
+        <v>65</v>
+      </c>
+      <c r="I59" s="109" t="s">
+        <v>46</v>
+      </c>
+      <c r="J59" s="109" t="s">
+        <v>55</v>
+      </c>
+      <c r="K59" s="111" t="s">
+        <v>46</v>
+      </c>
+      <c r="L59" s="138">
+        <v>2.08</v>
+      </c>
+      <c r="M59" s="75">
+        <f t="shared" si="2"/>
+        <v>66.56</v>
+      </c>
+      <c r="S59" s="167"/>
+      <c r="T59" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="60" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B60" s="112" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C60" s="113"/>
       <c r="D60" s="114">
@@ -4119,16 +4162,16 @@
       <c r="E60" s="114"/>
       <c r="F60" s="115"/>
       <c r="G60" s="115" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H60" s="116" t="s">
+        <v>62</v>
+      </c>
+      <c r="I60" s="115" t="s">
+        <v>28</v>
+      </c>
+      <c r="J60" s="115" t="s">
         <v>64</v>
-      </c>
-      <c r="I60" s="115" t="s">
-        <v>28</v>
-      </c>
-      <c r="J60" s="115" t="s">
-        <v>66</v>
       </c>
       <c r="K60" s="117" t="s">
         <v>28</v>
@@ -4142,9 +4185,9 @@
       </c>
       <c r="S60" s="167"/>
     </row>
-    <row r="61" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B61" s="112" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C61" s="113"/>
       <c r="D61" s="114">
@@ -4153,7 +4196,7 @@
       <c r="E61" s="114"/>
       <c r="F61" s="115"/>
       <c r="G61" s="115" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H61" s="116"/>
       <c r="I61" s="115"/>
@@ -4161,11 +4204,11 @@
       <c r="K61" s="117"/>
       <c r="L61" s="147"/>
       <c r="M61" s="81"/>
-      <c r="S61" s="195"/>
-    </row>
-    <row r="62" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S61" s="170"/>
+    </row>
+    <row r="62" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B62" s="70" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C62" s="108"/>
       <c r="D62" s="72">
@@ -4174,16 +4217,16 @@
       <c r="E62" s="72"/>
       <c r="F62" s="109"/>
       <c r="G62" s="109" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H62" s="110" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I62" s="109" t="s">
         <v>28</v>
       </c>
       <c r="J62" s="109" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K62" s="111" t="s">
         <v>28</v>
@@ -4197,9 +4240,9 @@
       </c>
       <c r="S62" s="167"/>
     </row>
-    <row r="63" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B63" s="112" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C63" s="113"/>
       <c r="D63" s="114">
@@ -4208,16 +4251,16 @@
       <c r="E63" s="114"/>
       <c r="F63" s="115"/>
       <c r="G63" s="115" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H63" s="116" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I63" s="115" t="s">
         <v>28</v>
       </c>
       <c r="J63" s="115" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="K63" s="117" t="s">
         <v>28</v>
@@ -4231,9 +4274,9 @@
       </c>
       <c r="S63" s="167"/>
     </row>
-    <row r="64" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B64" s="70" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C64" s="108"/>
       <c r="D64" s="72">
@@ -4242,16 +4285,16 @@
       <c r="E64" s="72"/>
       <c r="F64" s="109"/>
       <c r="G64" s="109" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H64" s="110" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I64" s="109" t="s">
         <v>28</v>
       </c>
       <c r="J64" s="109" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K64" s="111" t="s">
         <v>28</v>
@@ -4267,7 +4310,7 @@
     </row>
     <row r="65" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B65" s="112" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C65" s="116"/>
       <c r="D65" s="114">
@@ -4276,16 +4319,16 @@
       <c r="E65" s="114"/>
       <c r="F65" s="122"/>
       <c r="G65" s="122" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H65" s="116" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I65" s="115" t="s">
         <v>28</v>
       </c>
       <c r="J65" s="122" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K65" s="117" t="s">
         <v>28</v>
@@ -4301,7 +4344,7 @@
     </row>
     <row r="66" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B66" s="70" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C66" s="110"/>
       <c r="D66" s="72">
@@ -4310,16 +4353,16 @@
       <c r="E66" s="72"/>
       <c r="F66" s="74"/>
       <c r="G66" s="74" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H66" s="110" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I66" s="109" t="s">
         <v>28</v>
       </c>
       <c r="J66" s="74" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="K66" s="111" t="s">
         <v>28</v>
@@ -4335,7 +4378,7 @@
     </row>
     <row r="67" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B67" s="112" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C67" s="116"/>
       <c r="D67" s="114">
@@ -4344,16 +4387,16 @@
       <c r="E67" s="114"/>
       <c r="F67" s="122"/>
       <c r="G67" s="122" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H67" s="116" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I67" s="115" t="s">
         <v>28</v>
       </c>
       <c r="J67" s="122" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="K67" s="117" t="s">
         <v>28</v>
@@ -4369,7 +4412,7 @@
     </row>
     <row r="68" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B68" s="70" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C68" s="110"/>
       <c r="D68" s="72">
@@ -4378,16 +4421,16 @@
       <c r="E68" s="72"/>
       <c r="F68" s="74"/>
       <c r="G68" s="74" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H68" s="72" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I68" s="109" t="s">
         <v>28</v>
       </c>
       <c r="J68" s="74" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K68" s="111" t="s">
         <v>28</v>
@@ -4402,7 +4445,7 @@
     </row>
     <row r="69" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B69" s="64" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C69" s="123"/>
       <c r="D69" s="93">
@@ -4411,16 +4454,16 @@
       <c r="E69" s="93"/>
       <c r="F69" s="105"/>
       <c r="G69" s="105" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H69" s="93" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I69" s="124" t="s">
         <v>28</v>
       </c>
       <c r="J69" s="105" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="K69" s="125" t="s">
         <v>28</v>
@@ -4438,12 +4481,12 @@
       <c r="C70" s="4"/>
       <c r="F70" s="1"/>
       <c r="K70" s="148" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="L70" s="149"/>
       <c r="M70" s="150">
         <f>SUM(M48:M69)</f>
-        <v>267.892</v>
+        <v>355.67200000000003</v>
       </c>
     </row>
     <row r="71" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -4454,12 +4497,12 @@
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
       <c r="K72" s="148" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="L72" s="149"/>
       <c r="M72" s="150">
         <f>M40+M46+M70</f>
-        <v>1721.952</v>
+        <v>1812.932</v>
       </c>
     </row>
     <row r="73" spans="2:19" x14ac:dyDescent="0.2">
@@ -5336,6 +5379,19 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="D15:D16"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:D12"/>
@@ -5343,19 +5399,6 @@
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="D8:D10"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
@@ -5410,21 +5453,22 @@
     <hyperlink ref="K38" r:id="rId49" xr:uid="{1E7DE689-AB9F-4D10-A672-1396E98738D5}"/>
     <hyperlink ref="K35" r:id="rId50" xr:uid="{35ACFE45-5EC9-4D45-B080-718CB7702BA9}"/>
     <hyperlink ref="K36" r:id="rId51" xr:uid="{5CF4A831-3068-4205-B766-546D8134DAB7}"/>
+    <hyperlink ref="K59" r:id="rId52" xr:uid="{B270F44D-5DCA-4473-A1B5-4E0C4CABA102}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.118110236220472" right="0.196850393700787" top="0.16" bottom="0.25" header="0.11" footer="7.0000000000000007E-2"/>
-  <pageSetup paperSize="8" fitToWidth="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId52"/>
+  <pageSetup paperSize="8" fitToWidth="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId53"/>
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;CPage &amp;P of &amp;N&amp;R&amp;D  &amp;T</oddFooter>
   </headerFooter>
-  <drawing r:id="rId53"/>
-  <legacyDrawing r:id="rId54"/>
+  <drawing r:id="rId54"/>
+  <legacyDrawing r:id="rId55"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x14">
       <controls>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1030" r:id="rId55" name="AltiumMatBut">
+            <control shapeId="1030" r:id="rId56" name="AltiumMatBut">
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[1]!AltiumMatStart.AltiumMatStart">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
@@ -5446,7 +5490,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1031" r:id="rId56" name="Button 7">
+            <control shapeId="1031" r:id="rId57" name="Button 7">
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[1]!AltiumMan1ShowHide1" altText="Show/Hide ">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>

</xml_diff>